<commit_message>
g9 and 19 added
</commit_message>
<xml_diff>
--- a/Maintenance may june.xlsx
+++ b/Maintenance may june.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theho\Desktop\oxygengit\maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BAB66F-C519-44B0-9CB4-7D3EDF0454AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07598EAE-5BE9-43DA-9D4C-32F89AFB70F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="242">
   <si>
     <t xml:space="preserve">S.no </t>
   </si>
@@ -1788,8 +1788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C56038-014C-446F-8809-AF3D7B4BA2C5}">
   <dimension ref="A1:P96"/>
   <sheetViews>
-    <sheetView topLeftCell="B21" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2356,11 +2356,20 @@
         <v>6020</v>
       </c>
       <c r="K12" s="49">
-        <v>0</v>
+        <v>6020</v>
+      </c>
+      <c r="L12" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="M12" s="89" t="s">
+        <v>180</v>
+      </c>
+      <c r="N12" s="50" t="s">
+        <v>231</v>
       </c>
       <c r="O12" s="50">
         <f t="shared" si="0"/>
-        <v>6020</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
@@ -2824,11 +2833,20 @@
         <v>6292</v>
       </c>
       <c r="K22" s="49">
-        <v>0</v>
+        <v>6292</v>
+      </c>
+      <c r="L22" s="89" t="s">
+        <v>238</v>
+      </c>
+      <c r="M22" s="89" t="s">
+        <v>180</v>
+      </c>
+      <c r="N22" s="50" t="s">
+        <v>231</v>
       </c>
       <c r="O22" s="50">
         <f t="shared" si="0"/>
-        <v>6292</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:15" s="67" customFormat="1" x14ac:dyDescent="0.35">
@@ -5181,7 +5199,7 @@
       </c>
       <c r="K74" s="50">
         <f>SUM(K2:K73)</f>
-        <v>177638</v>
+        <v>189950</v>
       </c>
       <c r="L74" s="92"/>
       <c r="M74" s="92"/>
@@ -5299,8 +5317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F34115-B558-4DAE-88E2-CFCAD6F6585E}">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -5569,9 +5587,18 @@
       <c r="D12" s="109">
         <v>13104.333333333334</v>
       </c>
+      <c r="E12" s="107">
+        <v>13104.33</v>
+      </c>
       <c r="F12" s="114">
         <f t="shared" si="0"/>
-        <v>13104</v>
+        <v>0</v>
+      </c>
+      <c r="G12" s="107" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="107" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
@@ -5776,9 +5803,18 @@
       <c r="D22" s="109">
         <v>2089.3333333333335</v>
       </c>
+      <c r="E22" s="107">
+        <v>2089.33</v>
+      </c>
       <c r="F22" s="114">
         <f t="shared" si="0"/>
-        <v>2089</v>
+        <v>0</v>
+      </c>
+      <c r="G22" s="107" t="s">
+        <v>52</v>
+      </c>
+      <c r="H22" s="107" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
@@ -6859,7 +6895,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="134" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7022,8 +7058,8 @@
         <v>153</v>
       </c>
       <c r="C10">
-        <f>14965+11920</f>
-        <v>26885</v>
+        <f>14965+11920+19124+8381</f>
+        <v>54390</v>
       </c>
       <c r="D10" s="3">
         <f>79115+0</f>
@@ -7143,7 +7179,7 @@
       </c>
       <c r="C15" s="3">
         <f>SUM(C9:C14)</f>
-        <v>264550</v>
+        <v>292055</v>
       </c>
       <c r="D15" s="3">
         <f>SUM(D9:D14)</f>
@@ -7228,7 +7264,7 @@
   <dimension ref="A1:M88"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="134" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="L68" sqref="L68"/>
     </sheetView>
@@ -10261,7 +10297,7 @@
   <dimension ref="A1:V75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A44" sqref="A44:R44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
120 eb paid all clear
</commit_message>
<xml_diff>
--- a/Maintenance may june.xlsx
+++ b/Maintenance may june.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theho\Desktop\oxygengit\maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA274AE0-ABAF-4277-914B-E5C82C7C8A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA183B6-3D19-43C5-A37A-100490446692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="270">
   <si>
     <t xml:space="preserve">S.no </t>
   </si>
@@ -5888,7 +5888,7 @@
   <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -7414,9 +7414,18 @@
       <c r="D66" s="138">
         <v>794.33333333333303</v>
       </c>
+      <c r="E66" s="139">
+        <v>794</v>
+      </c>
       <c r="F66" s="139">
         <f t="shared" ref="F66:F72" si="2">ROUND(D66-E66,)</f>
-        <v>794</v>
+        <v>0</v>
+      </c>
+      <c r="G66" s="139" t="s">
+        <v>179</v>
+      </c>
+      <c r="H66" s="139" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.4">
@@ -7601,7 +7610,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7816,8 +7825,8 @@
         <v>202</v>
       </c>
       <c r="C12">
-        <f>7201+6591</f>
-        <v>13792</v>
+        <f>7201+6591+792</f>
+        <v>14584</v>
       </c>
       <c r="D12" s="53">
         <f>111280+0</f>
@@ -7887,7 +7896,7 @@
       </c>
       <c r="C15" s="53">
         <f>SUM(C9:C14)</f>
-        <v>317144</v>
+        <v>317936</v>
       </c>
       <c r="D15" s="53">
         <f>SUM(D9:D14)</f>

</xml_diff>

<commit_message>
may pay to residential and a missing diesel bill added
</commit_message>
<xml_diff>
--- a/Maintenance may june.xlsx
+++ b/Maintenance may june.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theho\Desktop\oxygengit\maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA183B6-3D19-43C5-A37A-100490446692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FDFCCF-AE3D-4A3A-A87E-2864C75ADF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="276">
   <si>
     <t xml:space="preserve">S.no </t>
   </si>
@@ -1014,6 +1014,24 @@
   <si>
     <t>only arrears cleared</t>
   </si>
+  <si>
+    <t xml:space="preserve">dg bill remaining </t>
+  </si>
+  <si>
+    <t>by Vishal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">part payment by anand on 22nd may </t>
+  </si>
+  <si>
+    <t>maintenance chunk paid to residential</t>
+  </si>
+  <si>
+    <t>by vishal</t>
+  </si>
+  <si>
+    <t>cash given</t>
+  </si>
 </sst>
 </file>
 
@@ -1022,7 +1040,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\ mmm\ yy"/>
   </numFmts>
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1292,6 +1310,21 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1391,7 +1424,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1739,6 +1772,11 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="6" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
@@ -2129,7 +2167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P96"/>
   <sheetViews>
-    <sheetView topLeftCell="C64" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C56" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P71" sqref="P71"/>
     </sheetView>
   </sheetViews>
@@ -5887,8 +5925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -7401,30 +7439,30 @@
         <v>794</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="139" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="137">
+    <row r="66" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="145">
         <v>120</v>
       </c>
-      <c r="B66" s="138">
-        <v>0</v>
-      </c>
-      <c r="C66" s="138">
+      <c r="B66" s="146">
+        <v>0</v>
+      </c>
+      <c r="C66" s="146">
         <v>794.33333333333303</v>
       </c>
-      <c r="D66" s="138">
+      <c r="D66" s="146">
         <v>794.33333333333303</v>
       </c>
-      <c r="E66" s="139">
+      <c r="E66" s="147">
         <v>794</v>
       </c>
-      <c r="F66" s="139">
+      <c r="F66" s="147">
         <f t="shared" ref="F66:F72" si="2">ROUND(D66-E66,)</f>
         <v>0</v>
       </c>
-      <c r="G66" s="139" t="s">
+      <c r="G66" s="147" t="s">
         <v>179</v>
       </c>
-      <c r="H66" s="139" t="s">
+      <c r="H66" s="147" t="s">
         <v>20</v>
       </c>
     </row>
@@ -7607,10 +7645,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7776,12 +7814,12 @@
         <v>198</v>
       </c>
       <c r="C10">
-        <f>14965+11920+19124+8381+3559+27044+12993+10600-8370+6528+1404+22200+2700+9530+11144+10000-13600-18348</f>
-        <v>131774</v>
+        <f>14965+11920+19124+8381+3559+27044+12993+10600-8370+6528+1404+22200+2700+9530+11144+10000-13600-18348-4941-70585</f>
+        <v>56248</v>
       </c>
       <c r="D10" s="53">
-        <f>79115+0</f>
-        <v>79115</v>
+        <f>79115-79115</f>
+        <v>0</v>
       </c>
       <c r="E10" s="57">
         <v>45761</v>
@@ -7896,11 +7934,11 @@
       </c>
       <c r="C15" s="53">
         <f>SUM(C9:C14)</f>
-        <v>317936</v>
+        <v>242410</v>
       </c>
       <c r="D15" s="53">
         <f>SUM(D9:D14)</f>
-        <v>190683</v>
+        <v>111568</v>
       </c>
       <c r="F15" t="s">
         <v>207</v>
@@ -7914,11 +7952,11 @@
       <c r="B16" s="53"/>
       <c r="C16" s="53"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B17" s="61"/>
       <c r="C17" s="61"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B18" s="53"/>
       <c r="C18" s="53"/>
       <c r="E18" s="57">
@@ -7934,7 +7972,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B19" s="53"/>
       <c r="C19" s="53"/>
       <c r="D19" s="61"/>
@@ -7951,7 +7989,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A20" s="63"/>
       <c r="B20" s="53"/>
       <c r="C20" s="53"/>
@@ -7968,7 +8006,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A21" s="63"/>
       <c r="B21" s="53"/>
       <c r="C21" s="53"/>
@@ -7985,7 +8023,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="63"/>
       <c r="B22" s="53"/>
       <c r="C22" s="53"/>
@@ -7996,13 +8034,13 @@
         <v>253</v>
       </c>
       <c r="G22">
-        <v>13699</v>
+        <v>13600</v>
       </c>
       <c r="H22" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B23" s="61"/>
       <c r="C23" s="61"/>
       <c r="E23" s="53" t="s">
@@ -8018,7 +8056,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E24" s="53" t="s">
         <v>258</v>
       </c>
@@ -8032,7 +8070,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E25" s="53" t="s">
         <v>264</v>
       </c>
@@ -8046,7 +8084,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E26" s="53" t="s">
         <v>264</v>
       </c>
@@ -8058,6 +8096,40 @@
       </c>
       <c r="H26" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E27" s="53" t="s">
+        <v>258</v>
+      </c>
+      <c r="F27" t="s">
+        <v>270</v>
+      </c>
+      <c r="G27">
+        <v>4941</v>
+      </c>
+      <c r="H27" t="s">
+        <v>271</v>
+      </c>
+      <c r="I27" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E28" s="53" t="s">
+        <v>250</v>
+      </c>
+      <c r="F28" t="s">
+        <v>273</v>
+      </c>
+      <c r="G28">
+        <v>149700</v>
+      </c>
+      <c r="H28" t="s">
+        <v>274</v>
+      </c>
+      <c r="I28" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>